<commit_message>
cambios al archivo de los ejercicios practica1
</commit_message>
<xml_diff>
--- a/practica1/RespuestaEjercicios1.xlsx
+++ b/practica1/RespuestaEjercicios1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>Entrada</t>
   </si>
@@ -27,23 +27,221 @@
     <t>Pasos</t>
   </si>
   <si>
-    <t>algoritmo</t>
-  </si>
-  <si>
-    <t>inicio</t>
-  </si>
-  <si>
-    <t>final</t>
-  </si>
-  <si>
     <t>Proceso</t>
+  </si>
+  <si>
+    <t>Ejercicio 1</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>1er numero</t>
+  </si>
+  <si>
+    <t>2do numero</t>
+  </si>
+  <si>
+    <t>3er numero</t>
+  </si>
+  <si>
+    <t>4to numero</t>
+  </si>
+  <si>
+    <t>5to numero</t>
+  </si>
+  <si>
+    <t>6to numero</t>
+  </si>
+  <si>
+    <t>7mo numero</t>
+  </si>
+  <si>
+    <t>8vo numero</t>
+  </si>
+  <si>
+    <t>9no numero</t>
+  </si>
+  <si>
+    <t>10mo numero</t>
+  </si>
+  <si>
+    <t>crear variable "resultado" para guardar el resultado de la suma.</t>
+  </si>
+  <si>
+    <t>Numeros ingresados ya sumados</t>
+  </si>
+  <si>
+    <t>Ejercicio 2</t>
+  </si>
+  <si>
+    <t>Leer numero, guardar en userNum.</t>
+  </si>
+  <si>
+    <t>crear array "vS[]" para guardar los numeros a sumar.</t>
+  </si>
+  <si>
+    <t>Leer 1er numero, guardar en vS[0].</t>
+  </si>
+  <si>
+    <t>Leer 2do numero, guardar en vS[1].</t>
+  </si>
+  <si>
+    <t>Leer 3er numero, guardar en vS[2].</t>
+  </si>
+  <si>
+    <t>Leer 4to numero, guardar en vS[3].</t>
+  </si>
+  <si>
+    <t>Leer 5to numero, guardar en vS[4].</t>
+  </si>
+  <si>
+    <t>Leer 6to numero, guardar en vS[5].</t>
+  </si>
+  <si>
+    <t>Leer 7mo numero, guardar en vS[6].</t>
+  </si>
+  <si>
+    <t>Leer 8vo numero, guardar en vS[7].</t>
+  </si>
+  <si>
+    <t>Leer 9no numero, guardar en vS[8].</t>
+  </si>
+  <si>
+    <t>Leer 10mo numero, guardar en vS[9].</t>
+  </si>
+  <si>
+    <t>resultado = vS[0] + vS[1] + vS[2] + vS[3] + vS[4] + vS[5] + vS[6] + vS[7] + vS[8] + vS[9].</t>
+  </si>
+  <si>
+    <t>fin.</t>
+  </si>
+  <si>
+    <t>Inicio.</t>
+  </si>
+  <si>
+    <t>numeros ingresados por el usuario.</t>
+  </si>
+  <si>
+    <t>guardar 2 en divisor.</t>
+  </si>
+  <si>
+    <t>crear constante divisor.</t>
+  </si>
+  <si>
+    <t>crear variable userNum.</t>
+  </si>
+  <si>
+    <t>crear variable resultado.</t>
+  </si>
+  <si>
+    <t>imprima resultado.</t>
+  </si>
+  <si>
+    <t>crear variable modCheck.</t>
+  </si>
+  <si>
+    <t>dividir userNum/2, guardar mod en modCheck.</t>
+  </si>
+  <si>
+    <t>si modCheck = 0, imprima "Es par".</t>
+  </si>
+  <si>
+    <t>Resultado de numero par</t>
+  </si>
+  <si>
+    <t>Ejercicio 3</t>
+  </si>
+  <si>
+    <t>numeros ingresado por el usuario.</t>
+  </si>
+  <si>
+    <t>Crear variable userNum.</t>
+  </si>
+  <si>
+    <t>Leer numero, guardarlo en userNum.</t>
+  </si>
+  <si>
+    <t>Ejercicio 4</t>
+  </si>
+  <si>
+    <t>1er numero del usuario</t>
+  </si>
+  <si>
+    <t>2do numero del usuario</t>
+  </si>
+  <si>
+    <t>3er numero del usuario</t>
+  </si>
+  <si>
+    <t>crear variable frstNum.</t>
+  </si>
+  <si>
+    <t>crear variable sndNum.</t>
+  </si>
+  <si>
+    <t>crear variable trdNum.</t>
+  </si>
+  <si>
+    <t>Leer 1er numero del usuario, guardar en frstNum.</t>
+  </si>
+  <si>
+    <t>Leer 3er numero del usuario, guardar en trdNum.</t>
+  </si>
+  <si>
+    <t>Leer 2do numero del usuario, guardar en sndNum.</t>
+  </si>
+  <si>
+    <t>crear variable highestNum.</t>
+  </si>
+  <si>
+    <t>si frstNum &lt;= sndNum, sndNum = highestNum.</t>
+  </si>
+  <si>
+    <t>sino frstNum = highestNum.</t>
+  </si>
+  <si>
+    <t>si highestNum &lt; trdNum, trdNum = resultado.</t>
+  </si>
+  <si>
+    <t>sino, highestNum = resultado.</t>
+  </si>
+  <si>
+    <t>El mayor de los tres numeros.</t>
+  </si>
+  <si>
+    <t>Ejercicio 5</t>
+  </si>
+  <si>
+    <t>crear constante zero que sea igual a 0.</t>
+  </si>
+  <si>
+    <t>crear variable num.</t>
+  </si>
+  <si>
+    <t>Leer numero, guardarlo en num.</t>
+  </si>
+  <si>
+    <t>si num != zero, imprimir num, volver al paso 4.</t>
+  </si>
+  <si>
+    <t>sino, ir al paso 7.</t>
+  </si>
+  <si>
+    <t>numeros diferentes a 0</t>
+  </si>
+  <si>
+    <t>Ejercicio 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +252,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,18 +294,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
+        <fgColor theme="6" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -114,27 +328,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,140 +710,835 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3" t="s">
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="12">
+        <v>2</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="12">
+        <v>3</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="12">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="12">
         <v>5</v>
       </c>
+      <c r="C26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="12">
+        <v>6</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="12">
+        <v>7</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="12">
+        <v>8</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="12">
+        <v>9</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="12">
+        <v>2</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="12">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="12">
+        <v>4</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="12">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="12">
+        <v>6</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="12">
+        <v>7</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="12">
+        <v>8</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="12">
+        <v>9</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>2</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>3</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="12">
+        <v>4</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="12">
+        <v>5</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="12">
+        <v>6</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="12">
+        <v>7</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="12">
+        <v>8</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="12">
+        <v>9</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="12">
+        <v>10</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="12">
+        <v>11</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="12">
+        <v>12</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="12">
+        <v>13</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="12">
+        <v>14</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="12">
+        <v>15</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>1</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="12">
+        <v>2</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="12">
+        <v>3</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="12">
+        <v>4</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="12">
+        <v>5</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="12">
+        <v>6</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="12">
+        <v>7</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="11"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>1</v>
+      </c>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="6"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="6"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A44:D44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ejercicios 7 8 comenzados
</commit_message>
<xml_diff>
--- a/practica1/RespuestaEjercicios1.xlsx
+++ b/practica1/RespuestaEjercicios1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="12345"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="102">
   <si>
     <t>Entrada</t>
   </si>
@@ -235,13 +235,100 @@
   </si>
   <si>
     <t>Ejercicio 6</t>
+  </si>
+  <si>
+    <t>Ejercicio 7</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Exponente</t>
+  </si>
+  <si>
+    <t>Elevar numero al exponente</t>
+  </si>
+  <si>
+    <t>Sino</t>
+  </si>
+  <si>
+    <t>Imprimir resultado</t>
+  </si>
+  <si>
+    <t>cont = cont + 1</t>
+  </si>
+  <si>
+    <t>resultado = num * exp</t>
+  </si>
+  <si>
+    <t>Si cont &lt;&gt; exp, entonces</t>
+  </si>
+  <si>
+    <t>cont = 1</t>
+  </si>
+  <si>
+    <t>Lee exp</t>
+  </si>
+  <si>
+    <t>Lee num</t>
+  </si>
+  <si>
+    <t>resultado = 0</t>
+  </si>
+  <si>
+    <t>Ir al paso 6</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>numeros</t>
+  </si>
+  <si>
+    <t>Suma de los pares</t>
+  </si>
+  <si>
+    <t>Suma de los impares</t>
+  </si>
+  <si>
+    <t>Sumar los numeros pares e impares ingresados por el usuario</t>
+  </si>
+  <si>
+    <t>Leer n</t>
+  </si>
+  <si>
+    <t>sino impar = impar + n.</t>
+  </si>
+  <si>
+    <t>si n mod 2 = 0, pares = pares + n.</t>
+  </si>
+  <si>
+    <t>pares = 0</t>
+  </si>
+  <si>
+    <t>impares = 0</t>
+  </si>
+  <si>
+    <t>Imprimir pares e impares</t>
+  </si>
+  <si>
+    <t>Sino, volver al paso 4</t>
+  </si>
+  <si>
+    <t>Si cont = 10 imprimir pares, impares, ir al paso 10</t>
+  </si>
+  <si>
+    <t>cont = 0</t>
+  </si>
+  <si>
+    <t>cont = cont +1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,8 +359,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,12 +378,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,8 +393,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -365,13 +466,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -379,18 +525,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,13 +546,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -710,834 +906,1453 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="74.5703125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="24">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="24">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="24">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="24">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="24">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="26">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="26">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="26">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="26">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="26">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="26">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="24">
         <v>1</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="12">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="25">
         <v>2</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="12">
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="25">
         <v>3</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="12">
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="25">
         <v>4</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="12">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="25">
         <v>5</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="12">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="25">
         <v>6</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="12">
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="25">
         <v>7</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="2"/>
+      <c r="D28" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="12">
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" s="25">
         <v>8</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="12">
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="25">
         <v>9</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="24">
         <v>1</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="12">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="25">
         <v>2</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="12">
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="25">
         <v>3</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="12">
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="25">
         <v>4</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="12">
+      <c r="C37" s="2"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="25">
         <v>5</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="12">
+      <c r="C38" s="2"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="25">
         <v>6</v>
       </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="12">
+      <c r="C39" s="2"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="25">
         <v>7</v>
       </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="12">
+      <c r="C40" s="2"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="25">
         <v>8</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="12">
+      <c r="C41" s="2"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="25">
         <v>9</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="2"/>
+      <c r="D42" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="24">
         <v>1</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="2"/>
+      <c r="D46" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="E46" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="24">
         <v>2</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="2"/>
+      <c r="D47" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="24">
         <v>3</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="12">
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="25">
         <v>4</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="2"/>
+      <c r="D49" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="12">
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="25">
         <v>5</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="2"/>
+      <c r="D50" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="6"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="12">
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="25">
         <v>6</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="2"/>
+      <c r="D51" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D51" s="6"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="12">
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B52" s="25">
         <v>7</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="6"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="12">
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="25">
         <v>8</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="2"/>
+      <c r="D53" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="12">
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="25">
         <v>9</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="2"/>
+      <c r="D54" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="12">
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="25">
         <v>10</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="2"/>
+      <c r="D55" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="12">
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="25">
         <v>11</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="2"/>
+      <c r="D56" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="12">
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="25">
         <v>12</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="2"/>
+      <c r="D57" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="12">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="25">
         <v>13</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="2"/>
+      <c r="D58" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="6"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="12">
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" s="25">
         <v>14</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="2"/>
+      <c r="D59" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="12">
+      <c r="E59" s="4"/>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="25">
         <v>15</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="2"/>
+      <c r="D60" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="E60" s="4"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="11"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="B62" s="9"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="10"/>
+    </row>
+    <row r="63" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="24">
         <v>1</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="2"/>
+      <c r="D64" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="E64" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="12">
+    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="25">
         <v>2</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="2"/>
+      <c r="D65" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D65" s="6"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="12">
+      <c r="E65" s="4"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="25">
         <v>3</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="2"/>
+      <c r="D66" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D66" s="6"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="12">
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B67" s="25">
         <v>4</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="2"/>
+      <c r="D67" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="6"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
-      <c r="B68" s="12">
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B68" s="25">
         <v>5</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="2"/>
+      <c r="D68" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="6"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
-      <c r="B69" s="12">
+      <c r="E68" s="4"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="25">
         <v>6</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="2"/>
+      <c r="D69" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="12">
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="25">
         <v>7</v>
       </c>
-      <c r="C70" s="14" t="s">
+      <c r="C70" s="2"/>
+      <c r="D70" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="E70" s="4"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="15"/>
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="11"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+    </row>
+    <row r="73" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="24">
         <v>1</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5" t="s">
+      <c r="B74" s="11"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D74" s="5"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="6"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="6"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="6"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="6"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="14"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="6"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="6"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" s="13"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B76" s="13"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B77" s="13"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" s="13"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" s="13"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" s="13"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
+        <v>87</v>
+      </c>
       <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" s="13"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83" s="13"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="13"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="13"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="20"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="24">
+        <v>1</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="24">
+        <v>2</v>
+      </c>
+      <c r="B91" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B92" s="24">
+        <v>3</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A93" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" s="24">
+        <v>4</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" s="24">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" s="24">
+        <v>6</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B96" s="24">
+        <v>6</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A97" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" s="24">
+        <v>6</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B98" s="24">
+        <v>7</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A99" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B99" s="24">
+        <v>8</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B100" s="24">
+        <v>8</v>
+      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B101" s="24">
+        <v>9</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="23"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="23"/>
+      <c r="E103" s="23"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D104" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="24">
+        <v>1</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C105" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B106" s="24">
+        <v>2</v>
+      </c>
+      <c r="C106" s="29"/>
+      <c r="D106" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B107" s="24">
+        <v>3</v>
+      </c>
+      <c r="C107" s="30"/>
+      <c r="D107" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B108" s="24">
+        <v>4</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B109" s="24">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110" s="24">
+        <v>6</v>
+      </c>
+      <c r="C110" s="2"/>
+      <c r="D110" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B111" s="24">
+        <v>7</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B112" s="24">
+        <v>8</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E112" s="4"/>
+    </row>
+    <row r="113" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" s="24">
+        <v>9</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E113" s="4"/>
+    </row>
+    <row r="114" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B114" s="24">
+        <v>10</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B115" s="26">
+        <v>11</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A116" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B116" s="26">
+        <v>12</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A88:E88"/>
+    <mergeCell ref="C105:C107"/>
     <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A72:D72"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A32:D32"/>
     <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A72:E72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>